<commit_message>
Figure, table, and markdown update
Adjusted figure and tables legends, and changes to supplementary methods to meet the EAU guidelines
</commit_message>
<xml_diff>
--- a/report/reviewer_tables.xlsx
+++ b/report/reviewer_tables.xlsx
@@ -427,9 +427,9 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BLCA: 90% (35)
-BLSC: 5.1% (2)
-UCU: 5.1% (2)
+          <t>BLCA: 35 (90)
+BLSC: 2 (5.1)
+UCU: 2 (5.1)
 complete: n = 39</t>
         </is>
       </c>
@@ -442,8 +442,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>66 [IQR: 57 - 80]
-range: 26 - 84
+          <t>66 (57, 80)
 complete: n = 24</t>
         </is>
       </c>
@@ -456,9 +455,9 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Female: 38% (15)
-Male: 56% (22)
-Unknown: 5.1% (2)
+          <t>Female: 15 (38)
+Male: 22 (56)
+Unknown: 2 (5.1)
 complete: n = 39</t>
         </is>
       </c>
@@ -471,7 +470,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>18% (7)
+          <t>7 (18)
 complete: n = 39</t>
         </is>
       </c>
@@ -482,13 +481,6 @@
           <t>Patient treatment status</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>pre-treatment: not available (0)
-post-treatment: not available (0)
-complete: n = 0</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -496,24 +488,11 @@
           <t>Systemic chemotherapy</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>not available (0)
-complete: n = 0</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
           <t>pT stage</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>T3: not available (0)
-T4: not available (0)
-complete: n = 0</t>
         </is>
       </c>
     </row>

</xml_diff>